<commit_message>
Added logos of Leiki and Sito to the front page. Fixed img alt tags.
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="150" yWindow="120" windowWidth="20730" windowHeight="11700" tabRatio="628" activeTab="1"/>
+    <workbookView xWindow="150" yWindow="120" windowWidth="20730" windowHeight="11700" tabRatio="628"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="12" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="688">
   <si>
     <t>fi</t>
   </si>
@@ -2187,6 +2187,18 @@
   </si>
   <si>
     <t>Aktivitetsvakten Tarkkailija har genomförts som en del av miljöministeriets projekt E-service för boende och byggande för produktion av elektroniska ärendehanterings- och informationstjänster i anslutning till boende och den byggda miljön. Projektet utgör en del av det program som finansministeriet inledde 2009 för att påskynda elektronisk ärendehantering och demokrati (SADe).</t>
+  </si>
+  <si>
+    <t>frontpage.leiki</t>
+  </si>
+  <si>
+    <t>Leiki</t>
+  </si>
+  <si>
+    <t>frontpage.sito</t>
+  </si>
+  <si>
+    <t>Sito</t>
   </si>
 </sst>
 </file>
@@ -2635,1699 +2647,1726 @@
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="169">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+  <dxfs count="171">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="170"/>
+      <tableStyleElement type="headerRow" dxfId="169"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4414,13 +4453,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>746125</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5815,10 +5854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C496"/>
+  <dimension ref="A1:C498"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6028,675 +6067,687 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>25</v>
+      <c r="A22" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>685</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>686</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>4</v>
+        <v>687</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>294</v>
-      </c>
+        <v>687</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
     </row>
     <row r="25" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>284</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>507</v>
+        <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>40</v>
+        <v>507</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>299</v>
+        <v>527</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>632</v>
+        <v>39</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>633</v>
+        <v>41</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>640</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>634</v>
+        <v>46</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>635</v>
+        <v>40</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>641</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>637</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>642</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>639</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>444</v>
+        <v>46</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>445</v>
+        <v>639</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>529</v>
+        <v>643</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>448</v>
+        <v>47</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>449</v>
+        <v>509</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>510</v>
+        <v>444</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>511</v>
+        <v>445</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B45" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>300</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>184</v>
+        <v>124</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>183</v>
+        <v>144</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>237</v>
+        <v>183</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>238</v>
+        <v>185</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>259</v>
+        <v>211</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>260</v>
+        <v>212</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="32.25" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>415</v>
+        <v>237</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>419</v>
+        <v>238</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>532</v>
+        <v>316</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>416</v>
+        <v>259</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>420</v>
+        <v>260</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>535</v>
+        <v>533</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>163</v>
+        <v>418</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>162</v>
+        <v>422</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>319</v>
+        <v>535</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>490</v>
+        <v>166</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>536</v>
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>492</v>
+        <v>170</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>489</v>
+        <v>171</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>537</v>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>131</v>
+        <v>492</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>132</v>
+        <v>489</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>323</v>
+        <v>537</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>485</v>
+        <v>134</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>538</v>
+        <v>323</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>155</v>
+        <v>485</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>326</v>
+        <v>538</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>397</v>
+        <v>154</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>398</v>
+        <v>155</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>402</v>
+        <v>326</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B87" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="116" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="5"/>
-      <c r="B116" s="6"/>
-      <c r="C116" s="6"/>
-    </row>
-    <row r="237" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="5"/>
-      <c r="B237" s="6"/>
-      <c r="C237" s="6"/>
-    </row>
-    <row r="267" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="1"/>
-      <c r="B267" s="9"/>
-      <c r="C267" s="6"/>
-    </row>
-    <row r="309" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A309" s="1"/>
-      <c r="B309" s="9"/>
-      <c r="C309" s="6"/>
-    </row>
-    <row r="327" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A327" s="5"/>
-      <c r="B327" s="6"/>
-      <c r="C327" s="6"/>
-    </row>
-    <row r="328" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A328" s="5"/>
-      <c r="B328" s="6"/>
-      <c r="C328" s="6"/>
+    <row r="118" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+    </row>
+    <row r="239" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="5"/>
+      <c r="B239" s="6"/>
+      <c r="C239" s="6"/>
+    </row>
+    <row r="269" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A269" s="1"/>
+      <c r="B269" s="9"/>
+      <c r="C269" s="6"/>
+    </row>
+    <row r="311" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A311" s="1"/>
+      <c r="B311" s="9"/>
+      <c r="C311" s="6"/>
     </row>
     <row r="329" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A329" s="5"/>
@@ -6733,15 +6784,15 @@
       <c r="B335" s="6"/>
       <c r="C335" s="6"/>
     </row>
-    <row r="340" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A340" s="5"/>
-      <c r="B340" s="6"/>
-      <c r="C340" s="6"/>
-    </row>
-    <row r="341" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A341" s="5"/>
-      <c r="B341" s="6"/>
-      <c r="C341" s="6"/>
+    <row r="336" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="5"/>
+      <c r="B336" s="6"/>
+      <c r="C336" s="6"/>
+    </row>
+    <row r="337" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="5"/>
+      <c r="B337" s="6"/>
+      <c r="C337" s="6"/>
     </row>
     <row r="342" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A342" s="5"/>
@@ -6753,47 +6804,47 @@
       <c r="B343" s="6"/>
       <c r="C343" s="6"/>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A350" s="5"/>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A351" s="5"/>
+    <row r="344" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="5"/>
+      <c r="B344" s="6"/>
+      <c r="C344" s="6"/>
+    </row>
+    <row r="345" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="5"/>
+      <c r="B345" s="6"/>
+      <c r="C345" s="6"/>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="5"/>
     </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B354" s="10"/>
-      <c r="C354" s="10"/>
-    </row>
-    <row r="380" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A380" s="1"/>
-      <c r="B380" s="9"/>
-      <c r="C380" s="6"/>
-    </row>
-    <row r="381" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A381" s="1"/>
-      <c r="B381" s="9"/>
-      <c r="C381" s="6"/>
-    </row>
-    <row r="387" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A387" s="5"/>
-      <c r="B387" s="6"/>
-      <c r="C387" s="6"/>
-    </row>
-    <row r="393" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A393" s="1"/>
-      <c r="B393" s="9"/>
-      <c r="C393" s="6"/>
-    </row>
-    <row r="394" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A394" s="5"/>
-      <c r="B394" s="6"/>
-      <c r="C394" s="6"/>
-    </row>
-    <row r="395" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A395" s="5"/>
-      <c r="B395" s="6"/>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" s="5"/>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" s="5"/>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B356" s="10"/>
+      <c r="C356" s="10"/>
+    </row>
+    <row r="382" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A382" s="1"/>
+      <c r="B382" s="9"/>
+      <c r="C382" s="6"/>
+    </row>
+    <row r="383" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A383" s="1"/>
+      <c r="B383" s="9"/>
+      <c r="C383" s="6"/>
+    </row>
+    <row r="389" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A389" s="5"/>
+      <c r="B389" s="6"/>
+      <c r="C389" s="6"/>
+    </row>
+    <row r="395" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A395" s="1"/>
+      <c r="B395" s="9"/>
       <c r="C395" s="6"/>
     </row>
     <row r="396" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6801,65 +6852,75 @@
       <c r="B396" s="6"/>
       <c r="C396" s="6"/>
     </row>
-    <row r="472" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A472" s="5"/>
-      <c r="B472" s="6"/>
-      <c r="C472" s="6"/>
-    </row>
-    <row r="473" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A473" s="4"/>
-      <c r="B473" s="6"/>
-      <c r="C473" s="6"/>
-    </row>
-    <row r="495" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A495" s="5"/>
-      <c r="B495" s="6"/>
-      <c r="C495" s="6"/>
-    </row>
-    <row r="496" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A496" s="5"/>
-      <c r="B496" s="6"/>
-      <c r="C496" s="6"/>
+    <row r="397" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A397" s="5"/>
+      <c r="B397" s="6"/>
+      <c r="C397" s="6"/>
+    </row>
+    <row r="398" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A398" s="5"/>
+      <c r="B398" s="6"/>
+      <c r="C398" s="6"/>
+    </row>
+    <row r="474" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A474" s="5"/>
+      <c r="B474" s="6"/>
+      <c r="C474" s="6"/>
+    </row>
+    <row r="475" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A475" s="4"/>
+      <c r="B475" s="6"/>
+      <c r="C475" s="6"/>
+    </row>
+    <row r="497" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A497" s="5"/>
+      <c r="B497" s="6"/>
+      <c r="C497" s="6"/>
+    </row>
+    <row r="498" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A498" s="5"/>
+      <c r="B498" s="6"/>
+      <c r="C498" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A158:A306 A308:A347 A87:A156 A7:A78 A1330:A1048576">
+  <conditionalFormatting sqref="A160:A308 A310:A349 A89:A158 A7:A80 A1332:A1048576">
     <cfRule type="expression" dxfId="168" priority="16">
       <formula>AND( $A7 = "", OR( $B7 &lt;&gt; "", $C7 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C158:C306 C308:C369 C1 C87:C156 C30:C32 C374:C1048576 C38:C62">
+  <conditionalFormatting sqref="C160:C308 C310:C371 C1 C89:C158 C32:C34 C40:C64 C376:C1048576">
     <cfRule type="expression" dxfId="167" priority="15">
       <formula>AND($B1 &lt;&gt; "", $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A157">
+  <conditionalFormatting sqref="A159">
     <cfRule type="expression" dxfId="166" priority="14">
-      <formula>AND( $A157 = "", OR( $B157 &lt;&gt; "", $C157 &lt;&gt; "" ) )</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C157">
+      <formula>AND( $A159 = "", OR( $B159 &lt;&gt; "", $C159 &lt;&gt; "" ) )</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C159">
     <cfRule type="expression" dxfId="165" priority="13">
-      <formula>AND($B157 &lt;&gt; "", $C157 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C370:C372">
+      <formula>AND($B159 &lt;&gt; "", $C159 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C372:C374">
     <cfRule type="expression" dxfId="164" priority="17">
-      <formula>AND($B371 &lt;&gt; "", $C370 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C373">
+      <formula>AND($B373 &lt;&gt; "", $C372 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C375">
     <cfRule type="expression" dxfId="163" priority="18">
-      <formula>AND(#REF! &lt;&gt; "", $C373 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A307">
+      <formula>AND(#REF! &lt;&gt; "", $C375 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A309">
     <cfRule type="expression" dxfId="162" priority="11">
-      <formula>AND( $A307 = "", OR( $B307 &lt;&gt; "", $C307 &lt;&gt; "" ) )</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C307">
+      <formula>AND( $A309 = "", OR( $B309 &lt;&gt; "", $C309 &lt;&gt; "" ) )</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C309">
     <cfRule type="expression" dxfId="161" priority="10">
-      <formula>AND($B307 &lt;&gt; "", $C307 = "")</formula>
+      <formula>AND($B309 &lt;&gt; "", $C309 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
@@ -6877,7 +6938,7 @@
       <formula>AND( $A3 = "", OR( $B3 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C15 C17:C29 C65">
+  <conditionalFormatting sqref="C7:C15 C17:C31 C67">
     <cfRule type="expression" dxfId="157" priority="6">
       <formula>AND($B7 &lt;&gt; "", $C7 = "")</formula>
     </cfRule>
@@ -6887,19 +6948,19 @@
       <formula>AND(#REF! &lt;&gt; "", $C4 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C66:C78">
+  <conditionalFormatting sqref="C68:C80">
     <cfRule type="expression" dxfId="155" priority="3">
-      <formula>AND($B66 &lt;&gt; "", $C66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+      <formula>AND($B68 &lt;&gt; "", $C68 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C87">
     <cfRule type="expression" dxfId="154" priority="2">
-      <formula>AND($B85 &lt;&gt; "", $C85 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33:C37">
+      <formula>AND($B87 &lt;&gt; "", $C87 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C39">
     <cfRule type="expression" dxfId="153" priority="1">
-      <formula>AND($B33 &lt;&gt; "", $C33 = "")</formula>
+      <formula>AND($B35 &lt;&gt; "", $C35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7863,8 +7924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>